<commit_message>
Specialty Staffing Final update
</commit_message>
<xml_diff>
--- a/TestData/TMTI0055029_VerifyInternalDealTeamSpecialtyRoleIncreasedLimitForCFLOBOpportunityEngagement.xlsx
+++ b/TestData/TMTI0055029_VerifyInternalDealTeamSpecialtyRoleIncreasedLimitForCFLOBOpportunityEngagement.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE511E96-3892-4F12-8D32-2E9A07D2C6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E8E0CB-30AF-402A-B102-76FC89FBECDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{2C05E2F5-3DB9-4FD8-8E59-14E5CD867A79}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C05E2F5-3DB9-4FD8-8E59-14E5CD867A79}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
-    <sheet name="Users" sheetId="2" r:id="rId2"/>
-    <sheet name="AddContact" sheetId="3" r:id="rId3"/>
-    <sheet name="OppDealTeamMembers" sheetId="4" r:id="rId4"/>
-    <sheet name="EngDealTeamMembers" sheetId="6" r:id="rId5"/>
-    <sheet name="OverlimitMessage" sheetId="5" r:id="rId6"/>
+    <sheet name="AppName" sheetId="7" r:id="rId2"/>
+    <sheet name="ModuleName" sheetId="8" r:id="rId3"/>
+    <sheet name="Users" sheetId="2" r:id="rId4"/>
+    <sheet name="AddContact" sheetId="3" r:id="rId5"/>
+    <sheet name="OppDealTeamMembers" sheetId="4" r:id="rId6"/>
+    <sheet name="EngDealTeamMembers" sheetId="6" r:id="rId7"/>
+    <sheet name="OverlimitMessage" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="103">
   <si>
     <t>Client</t>
   </si>
@@ -335,6 +337,21 @@
   </si>
   <si>
     <t>Jack Brodin</t>
+  </si>
+  <si>
+    <t>App Name</t>
+  </si>
+  <si>
+    <t>HL Banker</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>Opportunities</t>
   </si>
 </sst>
 </file>
@@ -378,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -391,7 +408,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1A1FE9-CADD-4FD6-8E73-186E076A589E}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,6 +920,67 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF1B31D-A2B0-43BC-A587-8474F3E673D9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FEA5EE-1EE6-46E7-A593-CB024A1C58ED}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7719AF-9118-4A60-BF7F-3491DAE91C27}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -938,12 +1015,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87197585-6EB4-40DD-9571-6763D8C561B1}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,12 +1087,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5D3C4F-7CA4-4B49-99BD-C542C86946E3}">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,7 +1161,7 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1114,7 +1191,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1159,7 +1236,7 @@
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="A28" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1169,11 +1246,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A1A452-25F2-430A-8358-9CDC08D43509}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1188,7 +1265,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1197,7 +1274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC13775-FB7E-4A2D-845E-DF647C6681C0}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>